<commit_message>
Tests databases and input files updated.
</commit_message>
<xml_diff>
--- a/tests/models/features/multi_intra_sets/input_data/input_data.xlsx
+++ b/tests/models/features/multi_intra_sets/input_data/input_data.xlsx
@@ -8,33 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\features\multi_intra_sets\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7F688C-D1EF-4EBC-B423-1EAC87AA476D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81667D9C-C7D1-4DBE-B722-4AA25998E353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2110" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dp" sheetId="4" r:id="rId1"/>
-    <sheet name="u" sheetId="5" r:id="rId2"/>
+    <sheet name="dp" sheetId="1" r:id="rId1"/>
+    <sheet name="u" sheetId="2" r:id="rId2"/>
     <sheet name="X" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dp!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">X!$A$1:$E$1</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -86,10 +69,10 @@
     <t>h5</t>
   </si>
   <si>
+    <t>s_Names</t>
+  </si>
+  <si>
     <t>y_Names</t>
-  </si>
-  <si>
-    <t>s_Names</t>
   </si>
   <si>
     <t>step</t>
@@ -460,11 +443,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6E5D7-19AA-434D-94F8-016B2D1BFF9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -997,28 +980,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3C4848-9BE6-49FC-A6A0-E5FA523562B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1127,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1138,10 +1112,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
@@ -1152,67 +1126,67 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>2020</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
         <v>2021</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>2022</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
       <c r="E4">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
         <v>2020</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -1220,401 +1194,396 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
         <v>2021</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
         <v>2022</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
       <c r="E7">
-        <v>300</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
         <v>2020</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
       <c r="E8">
-        <v>1000</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
         <v>2021</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
       <c r="E9">
-        <v>2000</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
         <v>2022</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
       <c r="E10">
-        <v>3000</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
         <v>2020</v>
       </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
       <c r="E11">
-        <v>20</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
         <v>2021</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
       <c r="E12">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
         <v>2022</v>
       </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
       <c r="E13">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
         <v>2020</v>
       </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
       <c r="E14">
-        <v>200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
         <v>2021</v>
       </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
       <c r="E15">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16">
         <v>2022</v>
       </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
       <c r="E16">
-        <v>600</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
         <v>2020</v>
       </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
       <c r="E17">
-        <v>2000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
         <v>2021</v>
       </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
       <c r="E18">
-        <v>4000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
         <v>2022</v>
       </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
       <c r="E19">
-        <v>6000</v>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
         <v>2020</v>
       </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
       <c r="E20">
-        <v>50</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
         <v>2021</v>
       </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
       <c r="E21">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
         <v>2022</v>
       </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
       <c r="E22">
-        <v>150</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
         <v>2020</v>
       </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
       <c r="E23">
-        <v>500</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
         <v>2021</v>
       </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
       <c r="E24">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25">
         <v>2022</v>
       </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
       <c r="E25">
-        <v>1500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>19</v>
       </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
         <v>2020</v>
       </c>
-      <c r="D26" t="s">
-        <v>17</v>
-      </c>
       <c r="E26">
-        <v>5000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
         <v>2021</v>
       </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
       <c r="E27">
-        <v>10000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28">
         <v>2022</v>
       </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
       <c r="E28">
-        <v>15000</v>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E28">
-      <sortCondition ref="D1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>